<commit_message>
removed glcode hierarchy to stuff would collapse properly
</commit_message>
<xml_diff>
--- a/Reports/TrialBalance_FromWarehouse_004.xlsx
+++ b/Reports/TrialBalance_FromWarehouse_004.xlsx
@@ -20,8 +20,8 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="60" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="52" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -29,7 +29,7 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{A2CB5862-8E78-49c6-8D9D-AF26E26ADB89}">
       <x15:timelineCachePivotCaches>
-        <pivotCache cacheId="4" r:id="rId5"/>
+        <pivotCache cacheId="5" r:id="rId5"/>
       </x15:timelineCachePivotCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}">
@@ -46,7 +46,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="._sql2012 Paga_BI" type="5" refreshedVersion="5" background="1" saveData="1">
+  <connection id="1" keepAlive="1" name="._sql2012 Paga_BI" type="5" refreshedVersion="5" background="1" refreshOnLoad="1" saveData="1">
     <dbPr connection="Provider=MSOLAP.6;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=Paga_BI;Data Source=.\sql2012;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error" command="Model" commandType="1"/>
     <olapPr sendLocale="1" rowDrillCount="1000"/>
   </connection>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Grand Total</t>
   </si>
@@ -93,18 +93,12 @@
     <t>General Ledger</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
     <t>LineItemCount</t>
   </si>
   <si>
-    <t>2015-03-05 18:10</t>
-  </si>
-  <si>
     <t>TxCount</t>
   </si>
   <si>
@@ -112,6 +106,126 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>2015-03-06 13:20</t>
+  </si>
+  <si>
+    <t>AGENT_BILL_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_DEPOSIT_TO_BANK_ACCOUNT</t>
+  </si>
+  <si>
+    <t>CUSTOMER_BILL_PAY</t>
+  </si>
+  <si>
+    <t>USER_DEPOSIT_FROM_BANK_ACCOUNT</t>
+  </si>
+  <si>
+    <t>USER_SEND_CASH_TO_BANK_ACCOUNT</t>
+  </si>
+  <si>
+    <t>AGENT_ACCEPT_DEPOSIT</t>
+  </si>
+  <si>
+    <t>AGENT_ACCEPT_DEPOSIT_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_BFS_ACCEPT_WITHDRAWAL</t>
+  </si>
+  <si>
+    <t>AGENT_BFS_COMMISSION</t>
+  </si>
+  <si>
+    <t>AGENT_BILL_PAY_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_BILL_PAY_FROM_STOCK</t>
+  </si>
+  <si>
+    <t>AGENT_DISPENSE_CASH_FOR_WITHDRAWAL_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_SELL_AIRTIME_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_SELL_AIRTIME_PRE_PAID</t>
+  </si>
+  <si>
+    <t>AGENT_SEND_CASH_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_SEND_CASH_CUSTOMER_TO_CUSTOMER</t>
+  </si>
+  <si>
+    <t>AGENT_SIGN_UP_CUSTOMER</t>
+  </si>
+  <si>
+    <t>AGENT_SIGN_UP_CUSTOMER_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>CUSTOMER_BILL_PAY_FROM_STOCK</t>
+  </si>
+  <si>
+    <t>PAGA_BFS_SETTLEMENT</t>
+  </si>
+  <si>
+    <t>PAGA_COLLECT_THIRD_PARTY_RECEIVABLES</t>
+  </si>
+  <si>
+    <t>PAGA_PAY_THIRD_PARTY_PAYABLE</t>
+  </si>
+  <si>
+    <t>USER_DEPOSIT_FROM_CARD</t>
+  </si>
+  <si>
+    <t>USER_DEPOSIT_FROM_CARD_FREE</t>
+  </si>
+  <si>
+    <t>AGENT_ACCEPT_DEPOSIT_COMMISSION</t>
+  </si>
+  <si>
+    <t>AGENT_BFS_ACCEPT_DEPOSIT</t>
+  </si>
+  <si>
+    <t>AGENT_BFS_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_DEPOSIT_TO_BANK_ACCOUNT_COMMISSION_PAY</t>
+  </si>
+  <si>
+    <t>BULK_PAY_AIRTIME_DISCOUNT_AWARD</t>
+  </si>
+  <si>
+    <t>BULK_PAY_BUY_AIRTIME_PRE_PAID</t>
+  </si>
+  <si>
+    <t>CUSTOMER_BUY_AIRTIME_PRE_PAID</t>
+  </si>
+  <si>
+    <t>CUSTOMER_REQUEST_WITHDRAW_CASH_REFUND</t>
+  </si>
+  <si>
+    <t>CUSTOMER_SEND_CASH_TO_CUSTOMER</t>
+  </si>
+  <si>
+    <t>CUSTOMER_SEND_CASH_TO_NONCUSTOMER</t>
+  </si>
+  <si>
+    <t>PAGA_HOLD_ACCOUNT_BALANCE</t>
+  </si>
+  <si>
+    <t>PAGA_PAY_BANK_WITHDRAW_TO_BANK_ACCOUNT_COMMISSION</t>
+  </si>
+  <si>
+    <t>PAGA_UNHOLD_ACCOUNT_BALANCE</t>
+  </si>
+  <si>
+    <t>USER_PREMIUM_SMS</t>
+  </si>
+  <si>
+    <t>USER_TRANSFER_FROM_CASH_BONUS_ACCOUNT</t>
   </si>
 </sst>
 </file>
@@ -154,42 +268,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="64">
     <dxf>
       <alignment horizontal="right" readingOrder="0"/>
     </dxf>
@@ -341,22 +437,40 @@
       <alignment horizontal="right" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" readingOrder="0"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" readingOrder="0"/>
@@ -454,17 +568,17 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42068.729620833336" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Christina Leo" refreshedDate="42069.578977893521" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="2">
     <cacheField name="[LatestFinancialTransaction].[LatestFinancialTx].[LatestFinancialTx]" caption="LatestFinancialTx" numFmtId="0" hierarchy="74" level="1">
       <sharedItems count="1">
-        <s v="[LatestFinancialTransaction].[LatestFinancialTx].&amp;[2015-03-05 18:10]" c="2015-03-05 18:10"/>
+        <s v="[LatestFinancialTransaction].[LatestFinancialTx].&amp;[2015-03-06 13:20]" c="2015-03-06 13:20"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Measures].[LineItemCount]" caption="LineItemCount" numFmtId="0" hierarchy="296" level="32767"/>
+    <cacheField name="[Measures].[LineItemCount]" caption="LineItemCount" numFmtId="0" hierarchy="303" level="32767"/>
   </cacheFields>
-  <cacheHierarchies count="320">
+  <cacheHierarchies count="330">
     <cacheHierarchy uniqueName="[BankingStatus].[BankingStatus]" caption="BankingStatus" attribute="1" defaultMemberUniqueName="[BankingStatus].[BankingStatus].[All]" allUniqueName="[BankingStatus].[BankingStatus].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[BankingStatus].[DimBankingStatusID]" caption="DimBankingStatusID" attribute="1" defaultMemberUniqueName="[BankingStatus].[DimBankingStatusID].[All]" allUniqueName="[BankingStatus].[DimBankingStatusID].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[Cancelled]" caption="Cancelled" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[Cancelled].[All]" allUniqueName="[FinancialTransaction].[Cancelled].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
@@ -744,6 +858,13 @@
     <cacheHierarchy uniqueName="[User].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[User].[Name].[All]" allUniqueName="[User].[Name].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[User].[RoleName]" caption="RoleName" attribute="1" defaultMemberUniqueName="[User].[RoleName].[All]" allUniqueName="[User].[RoleName].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[User].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[User].[SourceKey].[All]" allUniqueName="[User].[SourceKey].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[AccountNumber]" caption="AccountNumber" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[AccountNumber].[All]" allUniqueName="[FinancialHoldingAccount].[AccountNumber].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID]" caption="DimFinancialHoldingAccountID" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID].[All]" allUniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[Name].[All]" allUniqueName="[FinancialHoldingAccount].[Name].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[OpeningBalance]" caption="OpeningBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[OpeningBalance].[All]" allUniqueName="[FinancialHoldingAccount].[OpeningBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[RestrictedBalance].[All]" allUniqueName="[FinancialHoldingAccount].[RestrictedBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[SourceKey].[All]" allUniqueName="[FinancialHoldingAccount].[SourceKey].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[TotalBalance]" caption="TotalBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[TotalBalance].[All]" allUniqueName="[FinancialHoldingAccount].[TotalBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[DimFinancialTxTypeID]" caption="DimFinancialTxTypeID" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" allUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTxCategory]" caption="FinancialTxCategory" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" allUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[Name].[All]" allUniqueName="[FinancialTransactionType].[Name].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
@@ -771,6 +892,8 @@
         <fieldUsage x="1"/>
       </fieldsUsage>
     </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[OpeningBal]" caption="OpeningBal" measure="1" displayFolder="" measureGroup="GLCodeHierarchy" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[TotalBal]" caption="TotalBal" measure="1" displayFolder="" measureGroup="GLCodeHierarchy" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransactionType]" caption="_Count FinancialTransactionType" measure="1" displayFolder="" measureGroup="FinancialTransactionType" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransaction]" caption="_Count FinancialTransaction" measure="1" displayFolder="" measureGroup="FinancialTransaction" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count GLTransaction]" caption="_Count GLTransaction" measure="1" displayFolder="" measureGroup="GLTransaction" count="0" hidden="1"/>
@@ -793,6 +916,7 @@
     <cacheHierarchy uniqueName="[Measures].[_Count ProcessStartedDate]" caption="_Count ProcessStartedDate" measure="1" displayFolder="" measureGroup="ProcessStartedDate" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count PaymentUseCase]" caption="_Count PaymentUseCase" measure="1" displayFolder="" measureGroup="PaymentUseCase" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count LatestFinancialTransaction]" caption="_Count LatestFinancialTransaction" measure="1" displayFolder="" measureGroup="LatestFinancialTransaction" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count FinancialHoldingAccount]" caption="_Count FinancialHoldingAccount" measure="1" displayFolder="" measureGroup="FinancialHoldingAccount" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
   </cacheHierarchies>
   <kpis count="0"/>
@@ -821,8 +945,9 @@
     <dimension name="TransactionDate" uniqueName="[TransactionDate]" caption="TransactionDate"/>
     <dimension name="User" uniqueName="[User]" caption="User"/>
   </dimensions>
-  <measureGroups count="22">
+  <measureGroups count="23">
     <measureGroup name="BankingStatus" caption="BankingStatus"/>
+    <measureGroup name="FinancialHoldingAccount" caption="FinancialHoldingAccount"/>
     <measureGroup name="FinancialTransaction" caption="FinancialTransaction"/>
     <measureGroup name="FinancialTransactionType" caption="FinancialTransactionType"/>
     <measureGroup name="ForUser" caption="ForUser"/>
@@ -847,68 +972,68 @@
   </measureGroups>
   <maps count="63">
     <map measureGroup="0" dimension="0"/>
-    <map measureGroup="1" dimension="1"/>
-    <map measureGroup="1" dimension="2"/>
-    <map measureGroup="1" dimension="3"/>
-    <map measureGroup="1" dimension="6"/>
-    <map measureGroup="1" dimension="14"/>
-    <map measureGroup="1" dimension="15"/>
-    <map measureGroup="1" dimension="16"/>
-    <map measureGroup="1" dimension="17"/>
-    <map measureGroup="1" dimension="18"/>
-    <map measureGroup="1" dimension="19"/>
-    <map measureGroup="1" dimension="20"/>
-    <map measureGroup="1" dimension="21"/>
-    <map measureGroup="1" dimension="22"/>
+    <map measureGroup="2" dimension="1"/>
     <map measureGroup="2" dimension="2"/>
-    <map measureGroup="3" dimension="3"/>
-    <map measureGroup="4" dimension="4"/>
-    <map measureGroup="4" dimension="10"/>
-    <map measureGroup="4" dimension="11"/>
-    <map measureGroup="5" dimension="1"/>
-    <map measureGroup="5" dimension="2"/>
-    <map measureGroup="5" dimension="3"/>
+    <map measureGroup="2" dimension="3"/>
+    <map measureGroup="2" dimension="6"/>
+    <map measureGroup="2" dimension="14"/>
+    <map measureGroup="2" dimension="15"/>
+    <map measureGroup="2" dimension="16"/>
+    <map measureGroup="2" dimension="17"/>
+    <map measureGroup="2" dimension="18"/>
+    <map measureGroup="2" dimension="19"/>
+    <map measureGroup="2" dimension="20"/>
+    <map measureGroup="2" dimension="21"/>
+    <map measureGroup="2" dimension="22"/>
+    <map measureGroup="3" dimension="2"/>
+    <map measureGroup="4" dimension="3"/>
     <map measureGroup="5" dimension="4"/>
-    <map measureGroup="5" dimension="5"/>
-    <map measureGroup="5" dimension="6"/>
     <map measureGroup="5" dimension="10"/>
     <map measureGroup="5" dimension="11"/>
-    <map measureGroup="5" dimension="14"/>
-    <map measureGroup="5" dimension="15"/>
-    <map measureGroup="5" dimension="16"/>
-    <map measureGroup="5" dimension="17"/>
-    <map measureGroup="5" dimension="18"/>
-    <map measureGroup="5" dimension="19"/>
-    <map measureGroup="5" dimension="20"/>
-    <map measureGroup="5" dimension="21"/>
-    <map measureGroup="5" dimension="22"/>
+    <map measureGroup="6" dimension="1"/>
+    <map measureGroup="6" dimension="2"/>
+    <map measureGroup="6" dimension="3"/>
+    <map measureGroup="6" dimension="4"/>
+    <map measureGroup="6" dimension="5"/>
     <map measureGroup="6" dimension="6"/>
-    <map measureGroup="7" dimension="7"/>
-    <map measureGroup="8" dimension="9"/>
-    <map measureGroup="9" dimension="10"/>
-    <map measureGroup="9" dimension="11"/>
+    <map measureGroup="6" dimension="10"/>
+    <map measureGroup="6" dimension="11"/>
+    <map measureGroup="6" dimension="14"/>
+    <map measureGroup="6" dimension="15"/>
+    <map measureGroup="6" dimension="16"/>
+    <map measureGroup="6" dimension="17"/>
+    <map measureGroup="6" dimension="18"/>
+    <map measureGroup="6" dimension="19"/>
+    <map measureGroup="6" dimension="20"/>
+    <map measureGroup="6" dimension="21"/>
+    <map measureGroup="6" dimension="22"/>
+    <map measureGroup="7" dimension="6"/>
+    <map measureGroup="8" dimension="7"/>
+    <map measureGroup="9" dimension="9"/>
+    <map measureGroup="10" dimension="10"/>
     <map measureGroup="10" dimension="11"/>
-    <map measureGroup="11" dimension="12"/>
-    <map measureGroup="12" dimension="2"/>
-    <map measureGroup="12" dimension="13"/>
-    <map measureGroup="13" dimension="14"/>
-    <map measureGroup="14" dimension="15"/>
-    <map measureGroup="15" dimension="3"/>
-    <map measureGroup="15" dimension="6"/>
-    <map measureGroup="15" dimension="14"/>
+    <map measureGroup="11" dimension="11"/>
+    <map measureGroup="12" dimension="12"/>
+    <map measureGroup="13" dimension="2"/>
+    <map measureGroup="13" dimension="13"/>
+    <map measureGroup="14" dimension="14"/>
     <map measureGroup="15" dimension="15"/>
-    <map measureGroup="15" dimension="16"/>
-    <map measureGroup="15" dimension="17"/>
-    <map measureGroup="15" dimension="18"/>
-    <map measureGroup="15" dimension="19"/>
-    <map measureGroup="15" dimension="20"/>
-    <map measureGroup="15" dimension="22"/>
+    <map measureGroup="16" dimension="3"/>
+    <map measureGroup="16" dimension="6"/>
+    <map measureGroup="16" dimension="14"/>
+    <map measureGroup="16" dimension="15"/>
+    <map measureGroup="16" dimension="16"/>
     <map measureGroup="16" dimension="17"/>
-    <map measureGroup="17" dimension="18"/>
-    <map measureGroup="18" dimension="19"/>
-    <map measureGroup="19" dimension="20"/>
-    <map measureGroup="20" dimension="21"/>
-    <map measureGroup="21" dimension="22"/>
+    <map measureGroup="16" dimension="18"/>
+    <map measureGroup="16" dimension="19"/>
+    <map measureGroup="16" dimension="20"/>
+    <map measureGroup="16" dimension="22"/>
+    <map measureGroup="17" dimension="17"/>
+    <map measureGroup="18" dimension="18"/>
+    <map measureGroup="19" dimension="19"/>
+    <map measureGroup="20" dimension="20"/>
+    <map measureGroup="21" dimension="21"/>
+    <map measureGroup="22" dimension="22"/>
   </maps>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -919,69 +1044,70 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42069.323524189815" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Christina Leo" refreshedDate="42069.582805324077" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="13">
-    <cacheField name="[Measures].[Debits]" caption="Debits" numFmtId="0" hierarchy="290" level="32767"/>
-    <cacheField name="[Measures].[Credits]" caption="Credits" numFmtId="0" hierarchy="289" level="32767"/>
-    <cacheField name="[Measures].[Balance]" caption="Balance" numFmtId="0" hierarchy="291" level="32767"/>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[MainHeading]" caption="MainHeading" numFmtId="0" hierarchy="47" level="1">
-      <sharedItems count="2">
-        <s v="[GLCodeHierarchy].[GLCodes].[MainHeading].&amp;" c=""/>
-        <s v="[GLCodeHierarchy].[GLCodes].[MainHeading].&amp;[Chart of Accounts]" u="1" c="Chart of Accounts"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_1]" caption="SubHeading_1" numFmtId="0" hierarchy="47" level="2">
-      <sharedItems count="2">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_1].&amp;" c=""/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_1].&amp;[Assets]" u="1" c="Assets"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_2]" caption="SubHeading_2" numFmtId="0" hierarchy="47" level="3">
-      <sharedItems count="2">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;" c=""/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;[10100 - 19999:  Other Assets]" u="1" c="10100 - 19999:  Other Assets"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_3]" caption="SubHeading_3" numFmtId="0" hierarchy="47" level="4">
-      <sharedItems count="2">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;" c=""/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[13000 - 13999:  Banks]" u="1" c="13000 - 13999:  Banks"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_4]" caption="SubHeading_4" numFmtId="0" hierarchy="47" level="5">
-      <sharedItems count="2">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;" c=""/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[13110:  Pool Accounts]" u="1" c="13110:  Pool Accounts"/>
-      </sharedItems>
-    </cacheField>
+  <cacheFields count="7">
+    <cacheField name="[Measures].[Debits]" caption="Debits" numFmtId="0" hierarchy="297" level="32767"/>
+    <cacheField name="[Measures].[Credits]" caption="Credits" numFmtId="0" hierarchy="296" level="32767"/>
+    <cacheField name="[Measures].[Balance]" caption="Balance" numFmtId="0" hierarchy="298" level="32767"/>
     <cacheField name="[TransactionDate].[Date].[Date]" caption="Date" numFmtId="0" hierarchy="236" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[AccountType]" caption="AccountType" numFmtId="0" hierarchy="47" level="6">
-      <sharedItems count="3">
-        <s v="[GLCodeHierarchy].[GLCodes].[AccountType].&amp;" c=""/>
-        <s v="[GLCodeHierarchy].[GLCodes].[AccountType].&amp;[PAGA_POOL_ACCOUNT]" u="1" c="PAGA_POOL_ACCOUNT"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[AccountType].&amp;[PAGA_POOL_ACCOUNT_HOLDING_ACCOUNT]" u="1" c="PAGA_POOL_ACCOUNT_HOLDING_ACCOUNT"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[FinancialAccountID]" caption="FinancialAccountID" numFmtId="0" hierarchy="47" level="7">
-      <sharedItems count="1">
-        <s v="[GLCodeHierarchy].[GLCodes].[FinancialAccountID].&amp;" c=""/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Measures].[TxCount]" caption="TxCount" numFmtId="0" hierarchy="288" level="32767"/>
+    <cacheField name="[Measures].[TxCount]" caption="TxCount" numFmtId="0" hierarchy="295" level="32767"/>
     <cacheField name="[FinancialTransaction].[Cancelled].[Cancelled]" caption="Cancelled" numFmtId="0" hierarchy="2" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
+    <cacheField name="[FinancialTransactionType].[FinancialTransactionType].[FinancialTransactionType]" caption="FinancialTransactionType" numFmtId="0" hierarchy="26" level="1">
+      <sharedItems count="39">
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_ACCEPT_DEPOSIT]" c="AGENT_ACCEPT_DEPOSIT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_ACCEPT_DEPOSIT_COMMISSION]" c="AGENT_ACCEPT_DEPOSIT_COMMISSION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_ACCEPT_DEPOSIT_COMMISSION_PAY]" c="AGENT_ACCEPT_DEPOSIT_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BFS_ACCEPT_DEPOSIT]" c="AGENT_BFS_ACCEPT_DEPOSIT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BFS_ACCEPT_WITHDRAWAL]" c="AGENT_BFS_ACCEPT_WITHDRAWAL"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BFS_COMMISSION]" c="AGENT_BFS_COMMISSION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BFS_COMMISSION_PAY]" c="AGENT_BFS_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BILL_PAY]" c="AGENT_BILL_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BILL_PAY_COMMISSION_PAY]" c="AGENT_BILL_PAY_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BILL_PAY_FROM_STOCK]" c="AGENT_BILL_PAY_FROM_STOCK"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_DEPOSIT_TO_BANK_ACCOUNT]" c="AGENT_DEPOSIT_TO_BANK_ACCOUNT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_DEPOSIT_TO_BANK_ACCOUNT_COMMISSION_PAY]" c="AGENT_DEPOSIT_TO_BANK_ACCOUNT_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_DISPENSE_CASH_FOR_WITHDRAWAL_COMMISSION_PAY]" c="AGENT_DISPENSE_CASH_FOR_WITHDRAWAL_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SELL_AIRTIME_COMMISSION_PAY]" c="AGENT_SELL_AIRTIME_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SELL_AIRTIME_PRE_PAID]" c="AGENT_SELL_AIRTIME_PRE_PAID"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SEND_CASH_COMMISSION_PAY]" c="AGENT_SEND_CASH_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SEND_CASH_CUSTOMER_TO_CUSTOMER]" c="AGENT_SEND_CASH_CUSTOMER_TO_CUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SIGN_UP_CUSTOMER]" c="AGENT_SIGN_UP_CUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SIGN_UP_CUSTOMER_COMMISSION_PAY]" c="AGENT_SIGN_UP_CUSTOMER_COMMISSION_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[BULK_PAY_AIRTIME_DISCOUNT_AWARD]" c="BULK_PAY_AIRTIME_DISCOUNT_AWARD"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[BULK_PAY_BUY_AIRTIME_PRE_PAID]" c="BULK_PAY_BUY_AIRTIME_PRE_PAID"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_BILL_PAY]" c="CUSTOMER_BILL_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_BILL_PAY_FROM_STOCK]" c="CUSTOMER_BILL_PAY_FROM_STOCK"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_BUY_AIRTIME_PRE_PAID]" c="CUSTOMER_BUY_AIRTIME_PRE_PAID"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_REQUEST_WITHDRAW_CASH_REFUND]" c="CUSTOMER_REQUEST_WITHDRAW_CASH_REFUND"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_SEND_CASH_TO_CUSTOMER]" c="CUSTOMER_SEND_CASH_TO_CUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_SEND_CASH_TO_NONCUSTOMER]" c="CUSTOMER_SEND_CASH_TO_NONCUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_BFS_SETTLEMENT]" c="PAGA_BFS_SETTLEMENT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_COLLECT_THIRD_PARTY_RECEIVABLES]" c="PAGA_COLLECT_THIRD_PARTY_RECEIVABLES"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_HOLD_ACCOUNT_BALANCE]" c="PAGA_HOLD_ACCOUNT_BALANCE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_PAY_BANK_WITHDRAW_TO_BANK_ACCOUNT_COMMISSION]" c="PAGA_PAY_BANK_WITHDRAW_TO_BANK_ACCOUNT_COMMISSION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_PAY_THIRD_PARTY_PAYABLE]" c="PAGA_PAY_THIRD_PARTY_PAYABLE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_UNHOLD_ACCOUNT_BALANCE]" c="PAGA_UNHOLD_ACCOUNT_BALANCE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_DEPOSIT_FROM_BANK_ACCOUNT]" c="USER_DEPOSIT_FROM_BANK_ACCOUNT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_DEPOSIT_FROM_CARD]" c="USER_DEPOSIT_FROM_CARD"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_DEPOSIT_FROM_CARD_FREE]" c="USER_DEPOSIT_FROM_CARD_FREE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_PREMIUM_SMS]" c="USER_PREMIUM_SMS"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_SEND_CASH_TO_BANK_ACCOUNT]" c="USER_SEND_CASH_TO_BANK_ACCOUNT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_TRANSFER_FROM_CASH_BONUS_ACCOUNT]" c="USER_TRANSFER_FROM_CASH_BONUS_ACCOUNT"/>
+      </sharedItems>
+    </cacheField>
   </cacheFields>
-  <cacheHierarchies count="320">
+  <cacheHierarchies count="330">
     <cacheHierarchy uniqueName="[BankingStatus].[BankingStatus]" caption="BankingStatus" attribute="1" defaultMemberUniqueName="[BankingStatus].[BankingStatus].[All]" allUniqueName="[BankingStatus].[BankingStatus].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[BankingStatus].[DimBankingStatusID]" caption="DimBankingStatusID" attribute="1" defaultMemberUniqueName="[BankingStatus].[DimBankingStatusID].[All]" allUniqueName="[BankingStatus].[DimBankingStatusID].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[Cancelled]" caption="Cancelled" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[Cancelled].[All]" allUniqueName="[FinancialTransaction].[Cancelled].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="12"/>
+        <fieldUsage x="5"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[FinancialTransaction].[DimCurrencyID]" caption="DimCurrencyID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimCurrencyID].[All]" allUniqueName="[FinancialTransaction].[DimCurrencyID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
@@ -1005,9 +1131,14 @@
     <cacheHierarchy uniqueName="[FinancialTransaction].[ReferenceNumber]" caption="ReferenceNumber" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ReferenceNumber].[All]" allUniqueName="[FinancialTransaction].[ReferenceNumber].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[Reversed]" caption="Reversed" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[Reversed].[All]" allUniqueName="[FinancialTransaction].[Reversed].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[ShortCode]" caption="ShortCode" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ShortCode].[All]" allUniqueName="[FinancialTransaction].[ShortCode].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[FinancialTransaction].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[SourceKey].[All]" allUniqueName="[FinancialTransaction].[SourceKey].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[SourceKey].[All]" allUniqueName="[FinancialTransaction].[SourceKey].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[TextDescription]" caption="TextDescription" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[TextDescription].[All]" allUniqueName="[FinancialTransaction].[TextDescription].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTransactionType]" caption="FinancialTransactionType" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" allUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTransactionType]" caption="FinancialTransactionType" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" allUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="6"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[ForUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[ForUser].[DimCreatedDateID].[All]" allUniqueName="[ForUser].[DimCreatedDateID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[ForUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[ForUser].[DimDateOfBirthID].[All]" allUniqueName="[ForUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[ForUser].[DimForUserID]" caption="DimForUserID" attribute="1" defaultMemberUniqueName="[ForUser].[DimForUserID].[All]" allUniqueName="[ForUser].[DimForUserID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -1028,18 +1159,7 @@
     <cacheHierarchy uniqueName="[GLCodeHierarchy].[DimFinancialHoldingAccountID]" caption="DimFinancialHoldingAccountID" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[DimFinancialHoldingAccountID].[All]" allUniqueName="[GLCodeHierarchy].[DimFinancialHoldingAccountID].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[GLCodeHierarchy].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[DimPagaAccountID].[All]" allUniqueName="[GLCodeHierarchy].[DimPagaAccountID].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[GLCodeHierarchy].[FinancialAccountID]" caption="FinancialAccountID" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[FinancialAccountID].[All]" allUniqueName="[GLCodeHierarchy].[FinancialAccountID].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[GLCodeHierarchy].[GLCodes]" caption="GLCodes" defaultMemberUniqueName="[GLCodeHierarchy].[GLCodes].[All]" allUniqueName="[GLCodeHierarchy].[GLCodes].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="8" unbalanced="0">
-      <fieldsUsage count="8">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="3"/>
-        <fieldUsage x="4"/>
-        <fieldUsage x="5"/>
-        <fieldUsage x="6"/>
-        <fieldUsage x="7"/>
-        <fieldUsage x="9"/>
-        <fieldUsage x="10"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[GLCodes]" caption="GLCodes" defaultMemberUniqueName="[GLCodeHierarchy].[GLCodes].[All]" allUniqueName="[GLCodeHierarchy].[GLCodes].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="8" unbalanced="0"/>
     <cacheHierarchy uniqueName="[GLCodeHierarchy].[OpeningBalance]" caption="OpeningBalance" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[OpeningBalance].[All]" allUniqueName="[GLCodeHierarchy].[OpeningBalance].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[GLCodeHierarchy].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[RestrictedBalance].[All]" allUniqueName="[GLCodeHierarchy].[RestrictedBalance].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[GLCodeHierarchy].[TotalBalance]" caption="TotalBalance" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[TotalBalance].[All]" allUniqueName="[GLCodeHierarchy].[TotalBalance].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0"/>
@@ -1231,7 +1351,7 @@
     <cacheHierarchy uniqueName="[TransactionDate].[Date]" caption="Date" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[TransactionDate].[Date].[All]" allUniqueName="[TransactionDate].[Date].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="2" memberValueDatatype="7" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="8"/>
+        <fieldUsage x="3"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[TransactionDate].[DateID]" caption="DateID" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[DateID].[All]" allUniqueName="[TransactionDate].[DateID].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
@@ -1271,6 +1391,13 @@
     <cacheHierarchy uniqueName="[User].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[User].[Name].[All]" allUniqueName="[User].[Name].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[User].[RoleName]" caption="RoleName" attribute="1" defaultMemberUniqueName="[User].[RoleName].[All]" allUniqueName="[User].[RoleName].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[User].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[User].[SourceKey].[All]" allUniqueName="[User].[SourceKey].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[AccountNumber]" caption="AccountNumber" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[AccountNumber].[All]" allUniqueName="[FinancialHoldingAccount].[AccountNumber].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID]" caption="DimFinancialHoldingAccountID" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID].[All]" allUniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[Name].[All]" allUniqueName="[FinancialHoldingAccount].[Name].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[OpeningBalance]" caption="OpeningBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[OpeningBalance].[All]" allUniqueName="[FinancialHoldingAccount].[OpeningBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[RestrictedBalance].[All]" allUniqueName="[FinancialHoldingAccount].[RestrictedBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[SourceKey].[All]" allUniqueName="[FinancialHoldingAccount].[SourceKey].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[TotalBalance]" caption="TotalBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[TotalBalance].[All]" allUniqueName="[FinancialHoldingAccount].[TotalBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[DimFinancialTxTypeID]" caption="DimFinancialTxTypeID" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" allUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTxCategory]" caption="FinancialTxCategory" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" allUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[Name].[All]" allUniqueName="[FinancialTransactionType].[Name].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
@@ -1287,7 +1414,7 @@
     <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCaseType]" caption="PaymentUseCaseType" attribute="1" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCaseType].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCaseType].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[TxCount]" caption="TxCount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="11"/>
+        <fieldUsage x="4"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Credits]" caption="Credits" measure="1" displayFolder="" measureGroup="GLTransaction" count="0" oneField="1">
@@ -1310,6 +1437,8 @@
     <cacheHierarchy uniqueName="[Measures].[TxAmount]" caption="TxAmount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[ProcessTxAmt]" caption="ProcessTxAmt" measure="1" displayFolder="" measureGroup="ProcessEvent" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[LineItemCount]" caption="LineItemCount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[OpeningBal]" caption="OpeningBal" measure="1" displayFolder="" measureGroup="GLCodeHierarchy" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[TotalBal]" caption="TotalBal" measure="1" displayFolder="" measureGroup="GLCodeHierarchy" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransactionType]" caption="_Count FinancialTransactionType" measure="1" displayFolder="" measureGroup="FinancialTransactionType" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransaction]" caption="_Count FinancialTransaction" measure="1" displayFolder="" measureGroup="FinancialTransaction" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count GLTransaction]" caption="_Count GLTransaction" measure="1" displayFolder="" measureGroup="GLTransaction" count="0" hidden="1"/>
@@ -1332,6 +1461,7 @@
     <cacheHierarchy uniqueName="[Measures].[_Count ProcessStartedDate]" caption="_Count ProcessStartedDate" measure="1" displayFolder="" measureGroup="ProcessStartedDate" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count PaymentUseCase]" caption="_Count PaymentUseCase" measure="1" displayFolder="" measureGroup="PaymentUseCase" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count LatestFinancialTransaction]" caption="_Count LatestFinancialTransaction" measure="1" displayFolder="" measureGroup="LatestFinancialTransaction" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count FinancialHoldingAccount]" caption="_Count FinancialHoldingAccount" measure="1" displayFolder="" measureGroup="FinancialHoldingAccount" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
   </cacheHierarchies>
   <kpis count="0"/>
@@ -1360,8 +1490,9 @@
     <dimension name="TransactionDate" uniqueName="[TransactionDate]" caption="TransactionDate"/>
     <dimension name="User" uniqueName="[User]" caption="User"/>
   </dimensions>
-  <measureGroups count="22">
+  <measureGroups count="23">
     <measureGroup name="BankingStatus" caption="BankingStatus"/>
+    <measureGroup name="FinancialHoldingAccount" caption="FinancialHoldingAccount"/>
     <measureGroup name="FinancialTransaction" caption="FinancialTransaction"/>
     <measureGroup name="FinancialTransactionType" caption="FinancialTransactionType"/>
     <measureGroup name="ForUser" caption="ForUser"/>
@@ -1386,68 +1517,68 @@
   </measureGroups>
   <maps count="63">
     <map measureGroup="0" dimension="0"/>
-    <map measureGroup="1" dimension="1"/>
-    <map measureGroup="1" dimension="2"/>
-    <map measureGroup="1" dimension="3"/>
-    <map measureGroup="1" dimension="6"/>
-    <map measureGroup="1" dimension="14"/>
-    <map measureGroup="1" dimension="15"/>
-    <map measureGroup="1" dimension="16"/>
-    <map measureGroup="1" dimension="17"/>
-    <map measureGroup="1" dimension="18"/>
-    <map measureGroup="1" dimension="19"/>
-    <map measureGroup="1" dimension="20"/>
-    <map measureGroup="1" dimension="21"/>
-    <map measureGroup="1" dimension="22"/>
+    <map measureGroup="2" dimension="1"/>
     <map measureGroup="2" dimension="2"/>
-    <map measureGroup="3" dimension="3"/>
-    <map measureGroup="4" dimension="4"/>
-    <map measureGroup="4" dimension="10"/>
-    <map measureGroup="4" dimension="11"/>
-    <map measureGroup="5" dimension="1"/>
-    <map measureGroup="5" dimension="2"/>
-    <map measureGroup="5" dimension="3"/>
+    <map measureGroup="2" dimension="3"/>
+    <map measureGroup="2" dimension="6"/>
+    <map measureGroup="2" dimension="14"/>
+    <map measureGroup="2" dimension="15"/>
+    <map measureGroup="2" dimension="16"/>
+    <map measureGroup="2" dimension="17"/>
+    <map measureGroup="2" dimension="18"/>
+    <map measureGroup="2" dimension="19"/>
+    <map measureGroup="2" dimension="20"/>
+    <map measureGroup="2" dimension="21"/>
+    <map measureGroup="2" dimension="22"/>
+    <map measureGroup="3" dimension="2"/>
+    <map measureGroup="4" dimension="3"/>
     <map measureGroup="5" dimension="4"/>
-    <map measureGroup="5" dimension="5"/>
-    <map measureGroup="5" dimension="6"/>
     <map measureGroup="5" dimension="10"/>
     <map measureGroup="5" dimension="11"/>
-    <map measureGroup="5" dimension="14"/>
-    <map measureGroup="5" dimension="15"/>
-    <map measureGroup="5" dimension="16"/>
-    <map measureGroup="5" dimension="17"/>
-    <map measureGroup="5" dimension="18"/>
-    <map measureGroup="5" dimension="19"/>
-    <map measureGroup="5" dimension="20"/>
-    <map measureGroup="5" dimension="21"/>
-    <map measureGroup="5" dimension="22"/>
+    <map measureGroup="6" dimension="1"/>
+    <map measureGroup="6" dimension="2"/>
+    <map measureGroup="6" dimension="3"/>
+    <map measureGroup="6" dimension="4"/>
+    <map measureGroup="6" dimension="5"/>
     <map measureGroup="6" dimension="6"/>
-    <map measureGroup="7" dimension="7"/>
-    <map measureGroup="8" dimension="9"/>
-    <map measureGroup="9" dimension="10"/>
-    <map measureGroup="9" dimension="11"/>
+    <map measureGroup="6" dimension="10"/>
+    <map measureGroup="6" dimension="11"/>
+    <map measureGroup="6" dimension="14"/>
+    <map measureGroup="6" dimension="15"/>
+    <map measureGroup="6" dimension="16"/>
+    <map measureGroup="6" dimension="17"/>
+    <map measureGroup="6" dimension="18"/>
+    <map measureGroup="6" dimension="19"/>
+    <map measureGroup="6" dimension="20"/>
+    <map measureGroup="6" dimension="21"/>
+    <map measureGroup="6" dimension="22"/>
+    <map measureGroup="7" dimension="6"/>
+    <map measureGroup="8" dimension="7"/>
+    <map measureGroup="9" dimension="9"/>
+    <map measureGroup="10" dimension="10"/>
     <map measureGroup="10" dimension="11"/>
-    <map measureGroup="11" dimension="12"/>
-    <map measureGroup="12" dimension="2"/>
-    <map measureGroup="12" dimension="13"/>
-    <map measureGroup="13" dimension="14"/>
-    <map measureGroup="14" dimension="15"/>
-    <map measureGroup="15" dimension="3"/>
-    <map measureGroup="15" dimension="6"/>
-    <map measureGroup="15" dimension="14"/>
+    <map measureGroup="11" dimension="11"/>
+    <map measureGroup="12" dimension="12"/>
+    <map measureGroup="13" dimension="2"/>
+    <map measureGroup="13" dimension="13"/>
+    <map measureGroup="14" dimension="14"/>
     <map measureGroup="15" dimension="15"/>
-    <map measureGroup="15" dimension="16"/>
-    <map measureGroup="15" dimension="17"/>
-    <map measureGroup="15" dimension="18"/>
-    <map measureGroup="15" dimension="19"/>
-    <map measureGroup="15" dimension="20"/>
-    <map measureGroup="15" dimension="22"/>
+    <map measureGroup="16" dimension="3"/>
+    <map measureGroup="16" dimension="6"/>
+    <map measureGroup="16" dimension="14"/>
+    <map measureGroup="16" dimension="15"/>
+    <map measureGroup="16" dimension="16"/>
     <map measureGroup="16" dimension="17"/>
-    <map measureGroup="17" dimension="18"/>
-    <map measureGroup="18" dimension="19"/>
-    <map measureGroup="19" dimension="20"/>
-    <map measureGroup="20" dimension="21"/>
-    <map measureGroup="21" dimension="22"/>
+    <map measureGroup="16" dimension="18"/>
+    <map measureGroup="16" dimension="19"/>
+    <map measureGroup="16" dimension="20"/>
+    <map measureGroup="16" dimension="22"/>
+    <map measureGroup="17" dimension="17"/>
+    <map measureGroup="18" dimension="18"/>
+    <map measureGroup="19" dimension="19"/>
+    <map measureGroup="20" dimension="20"/>
+    <map measureGroup="21" dimension="21"/>
+    <map measureGroup="22" dimension="22"/>
   </maps>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -1458,7 +1589,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42068.729606712965" backgroundQuery="1" createdVersion="3" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Christina Leo" refreshedDate="42069.578554861109" backgroundQuery="1" createdVersion="3" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1">
     <extLst>
       <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
@@ -1467,7 +1598,7 @@
     </extLst>
   </cacheSource>
   <cacheFields count="0"/>
-  <cacheHierarchies count="320">
+  <cacheHierarchies count="330">
     <cacheHierarchy uniqueName="[BankingStatus].[BankingStatus]" caption="BankingStatus" attribute="1" defaultMemberUniqueName="[BankingStatus].[BankingStatus].[All]" allUniqueName="[BankingStatus].[BankingStatus].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[BankingStatus].[DimBankingStatusID]" caption="DimBankingStatusID" attribute="1" defaultMemberUniqueName="[BankingStatus].[DimBankingStatusID].[All]" allUniqueName="[BankingStatus].[DimBankingStatusID].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[Cancelled]" caption="Cancelled" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[Cancelled].[All]" allUniqueName="[FinancialTransaction].[Cancelled].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
@@ -1742,6 +1873,13 @@
     <cacheHierarchy uniqueName="[User].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[User].[Name].[All]" allUniqueName="[User].[Name].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[User].[RoleName]" caption="RoleName" attribute="1" defaultMemberUniqueName="[User].[RoleName].[All]" allUniqueName="[User].[RoleName].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[User].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[User].[SourceKey].[All]" allUniqueName="[User].[SourceKey].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[AccountNumber]" caption="AccountNumber" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[AccountNumber].[All]" allUniqueName="[FinancialHoldingAccount].[AccountNumber].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID]" caption="DimFinancialHoldingAccountID" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID].[All]" allUniqueName="[FinancialHoldingAccount].[DimFinancialHoldingAccountID].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[Name].[All]" allUniqueName="[FinancialHoldingAccount].[Name].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[OpeningBalance]" caption="OpeningBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[OpeningBalance].[All]" allUniqueName="[FinancialHoldingAccount].[OpeningBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[RestrictedBalance].[All]" allUniqueName="[FinancialHoldingAccount].[RestrictedBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[SourceKey].[All]" allUniqueName="[FinancialHoldingAccount].[SourceKey].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialHoldingAccount].[TotalBalance]" caption="TotalBalance" attribute="1" defaultMemberUniqueName="[FinancialHoldingAccount].[TotalBalance].[All]" allUniqueName="[FinancialHoldingAccount].[TotalBalance].[All]" dimensionUniqueName="[FinancialHoldingAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[DimFinancialTxTypeID]" caption="DimFinancialTxTypeID" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" allUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTxCategory]" caption="FinancialTxCategory" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" allUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[FinancialTransactionType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[Name].[All]" allUniqueName="[FinancialTransactionType].[Name].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
@@ -1765,6 +1903,8 @@
     <cacheHierarchy uniqueName="[Measures].[TxAmount]" caption="TxAmount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[ProcessTxAmt]" caption="ProcessTxAmt" measure="1" displayFolder="" measureGroup="ProcessEvent" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[LineItemCount]" caption="LineItemCount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[OpeningBal]" caption="OpeningBal" measure="1" displayFolder="" measureGroup="GLCodeHierarchy" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[TotalBal]" caption="TotalBal" measure="1" displayFolder="" measureGroup="GLCodeHierarchy" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransactionType]" caption="_Count FinancialTransactionType" measure="1" displayFolder="" measureGroup="FinancialTransactionType" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransaction]" caption="_Count FinancialTransaction" measure="1" displayFolder="" measureGroup="FinancialTransaction" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count GLTransaction]" caption="_Count GLTransaction" measure="1" displayFolder="" measureGroup="GLTransaction" count="0" hidden="1"/>
@@ -1787,12 +1927,13 @@
     <cacheHierarchy uniqueName="[Measures].[_Count ProcessStartedDate]" caption="_Count ProcessStartedDate" measure="1" displayFolder="" measureGroup="ProcessStartedDate" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count PaymentUseCase]" caption="_Count PaymentUseCase" measure="1" displayFolder="" measureGroup="PaymentUseCase" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count LatestFinancialTransaction]" caption="_Count LatestFinancialTransaction" measure="1" displayFolder="" measureGroup="LatestFinancialTransaction" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count FinancialHoldingAccount]" caption="_Count FinancialHoldingAccount" measure="1" displayFolder="" measureGroup="FinancialHoldingAccount" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
   </cacheHierarchies>
   <kpis count="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition pivotCacheId="23" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+      <x14:pivotCacheDefinition pivotCacheId="25" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{ABF5C744-AB39-4b91-8756-CFA1BBC848D5}">
       <x15:pivotCacheIdVersion cacheIdSupportedVersion="6" cacheIdCreatedVersion="6"/>
@@ -1802,68 +1943,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="60" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="5" subtotalHiddenItems="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="General Ledger" colHeaderCaption="Transactions Available Through" fieldListSortAscending="1">
-  <location ref="B23:F31" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="5" subtotalHiddenItems="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="General Ledger" colHeaderCaption="Transactions Available Through" fieldListSortAscending="1">
+  <location ref="B23:F63" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1">
-      <items count="3">
-        <item s="1" c="1" x="0" d="1"/>
-        <item x="1" d="1"/>
-        <item t="default"/>
-      </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="3">
-        <item c="1" x="0" d="1"/>
-        <item x="1" d="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="3">
-        <item c="1" x="0" d="1"/>
-        <item x="1" d="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="3">
-        <item c="1" x="0" d="1"/>
-        <item x="1" d="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="3">
-        <item c="1" x="0" d="1"/>
-        <item x="1" d="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="1">
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" hideNewItems="1" dataSourceSort="1">
-      <items count="4">
-        <item c="1" x="0" d="1"/>
-        <item x="1" d="1"/>
-        <item x="2" d="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" hideNewItems="1" dataSourceSort="1">
-      <items count="2">
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1873,37 +1960,171 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField axis="axisRow" allDrilled="1" outline="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="40">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowFields count="7">
-    <field x="3"/>
-    <field x="4"/>
-    <field x="5"/>
+  <rowFields count="1">
     <field x="6"/>
-    <field x="7"/>
-    <field x="9"/>
-    <field x="10"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="40">
     <i>
       <x/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="4">
-      <x/>
-    </i>
-    <i r="5">
-      <x/>
-    </i>
-    <i r="6">
-      <x/>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
     </i>
     <i t="grand">
       <x/>
@@ -1927,16 +2148,16 @@
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="12" hier="2" name="[FinancialTransaction].[Cancelled].&amp;[False]" cap="False"/>
+    <pageField fld="5" hier="2" name="[FinancialTransaction].[Cancelled].&amp;[False]" cap="False"/>
   </pageFields>
   <dataFields count="4">
     <dataField fld="0" baseField="0" baseItem="0" numFmtId="4"/>
     <dataField fld="1" baseField="0" baseItem="0" numFmtId="4"/>
     <dataField fld="2" baseField="0" baseItem="0" numFmtId="4"/>
-    <dataField fld="11" baseField="3" baseItem="1" numFmtId="3"/>
+    <dataField fld="4" baseField="3" baseItem="1" numFmtId="3"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="0">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1945,7 +2166,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -1955,7 +2176,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="61">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1964,7 +2185,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1974,7 +2195,7 @@
       </pivotArea>
     </format>
   </formats>
-  <pivotHierarchies count="320">
+  <pivotHierarchies count="330">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy multipleItemSelectionAllowed="1">
@@ -2267,6 +2488,16 @@
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
@@ -2302,7 +2533,7 @@
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <filters count="1">
-    <filter fld="8" type="dateEqual" evalOrder="-1" id="21" name="[TransactionDate].[Date]">
+    <filter fld="3" type="dateEqual" evalOrder="-1" id="24" name="[TransactionDate].[Date]">
       <autoFilter ref="A1">
         <filterColumn colId="0">
           <customFilters>
@@ -2318,7 +2549,7 @@
     </filter>
   </filters>
   <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="47"/>
+    <rowHierarchyUsage hierarchyUsage="26"/>
   </rowHierarchiesUsage>
   <colHierarchiesUsage count="1">
     <colHierarchyUsage hierarchyUsage="-2"/>
@@ -2332,7 +2563,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
@@ -2360,295 +2591,305 @@
   <dataFields count="1">
     <dataField fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="320">
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
+  <pivotHierarchies count="330">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
@@ -2960,7 +3201,7 @@
   <pivotTables>
     <pivotTable tabId="1" name="PivotTable1"/>
   </pivotTables>
-  <state minimalRefreshVersion="6" lastRefreshVersion="6" pivotCacheId="23" filterType="dateEqual">
+  <state minimalRefreshVersion="6" lastRefreshVersion="6" pivotCacheId="25" filterType="dateEqual">
     <selection startDate="2015-01-01T00:00:00" endDate="2015-01-01T00:00:00"/>
     <bounds startDate="2010-01-01T00:00:00" endDate="2016-01-01T00:00:00"/>
   </state>
@@ -2975,10 +3216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B10:F31"/>
+  <dimension ref="B10:F63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2989,168 +3230,714 @@
   </cols>
   <sheetData>
     <row r="10" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="str">
+      <c r="B10" s="5" t="str">
         <f>"Data Available through:  " &amp;Sheet2!A2</f>
-        <v>Data Available through:  2015-03-05 18:10</v>
+        <v>Data Available through:  2015-03-06 13:20</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s" vm="1">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>9</v>
+      <c r="F23" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2374044.7800000003</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2374044.7799999998</v>
+      </c>
+      <c r="E24" s="3">
         <v>0</v>
       </c>
-      <c r="D24" s="5">
+      <c r="F24" s="7">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="3">
+        <v>7980</v>
+      </c>
+      <c r="D25" s="3">
+        <v>7980</v>
+      </c>
+      <c r="E25" s="3">
         <v>0</v>
       </c>
-      <c r="E24" s="5">
+      <c r="F25" s="7">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1562720</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1562720</v>
+      </c>
+      <c r="E26" s="3">
         <v>0</v>
       </c>
-      <c r="F24" s="13">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="F26" s="7">
+        <v>13784</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="3">
+        <v>5500</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5500</v>
+      </c>
+      <c r="E27" s="3">
         <v>0</v>
       </c>
-      <c r="D25" s="5">
+      <c r="F27" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="3">
+        <v>5000</v>
+      </c>
+      <c r="D28" s="3">
+        <v>5000</v>
+      </c>
+      <c r="E28" s="3">
         <v>0</v>
       </c>
-      <c r="E25" s="5">
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="3">
+        <v>39105.5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>39105.5</v>
+      </c>
+      <c r="E29" s="3">
         <v>0</v>
       </c>
-      <c r="F25" s="13">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="F29" s="7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3">
+        <v>44112.099999999955</v>
+      </c>
+      <c r="D30" s="3">
+        <v>44112.100000000006</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4.2206238504149951E-12</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="3">
+        <v>6354650</v>
+      </c>
+      <c r="D31" s="3">
+        <v>6354650.0000000019</v>
+      </c>
+      <c r="E31" s="3">
+        <v>-1.3387762010097504E-9</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3318</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="3">
+        <v>8171828.75</v>
+      </c>
+      <c r="D32" s="3">
+        <v>8171828.75</v>
+      </c>
+      <c r="E32" s="3">
         <v>0</v>
       </c>
-      <c r="D26" s="5">
+      <c r="F32" s="7">
+        <v>294520</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1340500</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1340500</v>
+      </c>
+      <c r="E33" s="3">
         <v>0</v>
       </c>
-      <c r="E26" s="5">
+      <c r="F33" s="7">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3213584</v>
+      </c>
+      <c r="D34" s="3">
+        <v>3213584</v>
+      </c>
+      <c r="E34" s="3">
         <v>0</v>
       </c>
-      <c r="F26" s="13">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="F34" s="7">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2770360</v>
+      </c>
+      <c r="D35" s="3">
+        <v>2770360</v>
+      </c>
+      <c r="E35" s="3">
         <v>0</v>
       </c>
-      <c r="D27" s="5">
+      <c r="F35" s="7">
+        <v>42833</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="3">
+        <v>130320</v>
+      </c>
+      <c r="D36" s="3">
+        <v>130320</v>
+      </c>
+      <c r="E36" s="3">
         <v>0</v>
       </c>
-      <c r="E27" s="5">
+      <c r="F36" s="7">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1803601.7599999998</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1803601.7599999998</v>
+      </c>
+      <c r="E37" s="3">
+        <v>-2.1827872842550278E-10</v>
+      </c>
+      <c r="F37" s="7">
+        <v>84693</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="3">
+        <v>938861.11999999988</v>
+      </c>
+      <c r="D38" s="3">
+        <v>938861.13000000012</v>
+      </c>
+      <c r="E38" s="3">
+        <v>-1.0000000156651367E-2</v>
+      </c>
+      <c r="F38" s="7">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="3">
+        <v>11400</v>
+      </c>
+      <c r="D39" s="3">
+        <v>11400</v>
+      </c>
+      <c r="E39" s="3">
         <v>0</v>
       </c>
-      <c r="F27" s="13">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="F39" s="7">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="3">
+        <v>5150</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5150</v>
+      </c>
+      <c r="E40" s="3">
         <v>0</v>
       </c>
-      <c r="D28" s="5">
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="3">
+        <v>150</v>
+      </c>
+      <c r="D41" s="3">
+        <v>150</v>
+      </c>
+      <c r="E41" s="3">
         <v>0</v>
       </c>
-      <c r="E28" s="5">
+      <c r="F41" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="3">
+        <v>8700</v>
+      </c>
+      <c r="D42" s="3">
+        <v>8700</v>
+      </c>
+      <c r="E42" s="3">
         <v>0</v>
       </c>
-      <c r="F28" s="13">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="F42" s="7">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="3">
+        <v>905</v>
+      </c>
+      <c r="D43" s="3">
+        <v>905</v>
+      </c>
+      <c r="E43" s="3">
         <v>0</v>
       </c>
-      <c r="D29" s="5">
+      <c r="F43" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="3">
+        <v>90500</v>
+      </c>
+      <c r="D44" s="3">
+        <v>90500</v>
+      </c>
+      <c r="E44" s="3">
         <v>0</v>
       </c>
-      <c r="E29" s="5">
+      <c r="F44" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="3">
+        <v>3127205.63</v>
+      </c>
+      <c r="D45" s="3">
+        <v>3127205.6400000015</v>
+      </c>
+      <c r="E45" s="3">
+        <v>-1.0000001610478648E-2</v>
+      </c>
+      <c r="F45" s="7">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="3">
+        <v>8980</v>
+      </c>
+      <c r="D46" s="3">
+        <v>8980</v>
+      </c>
+      <c r="E46" s="3">
         <v>0</v>
       </c>
-      <c r="F29" s="13">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="C30" s="5">
+      <c r="F46" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="3">
+        <v>168421.81</v>
+      </c>
+      <c r="D47" s="3">
+        <v>168421.81</v>
+      </c>
+      <c r="E47" s="3">
+        <v>3.637978807091713E-12</v>
+      </c>
+      <c r="F47" s="7">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1070</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1070</v>
+      </c>
+      <c r="E48" s="3">
         <v>0</v>
       </c>
-      <c r="D30" s="5">
+      <c r="F48" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1595205.42</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1595205.42</v>
+      </c>
+      <c r="E49" s="3">
+        <v>-1.1641532182693481E-10</v>
+      </c>
+      <c r="F49" s="7">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1100</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1100</v>
+      </c>
+      <c r="E50" s="3">
         <v>0</v>
       </c>
-      <c r="E30" s="5">
+      <c r="F50" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="3">
+        <v>49600</v>
+      </c>
+      <c r="D51" s="3">
+        <v>49600</v>
+      </c>
+      <c r="E51" s="3">
         <v>0</v>
       </c>
-      <c r="F30" s="13">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="F51" s="7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="3">
+        <v>6044182.5000000009</v>
+      </c>
+      <c r="D52" s="3">
+        <v>6044182.5000000009</v>
+      </c>
+      <c r="E52" s="3">
+        <v>-1.4551915228366852E-10</v>
+      </c>
+      <c r="F52" s="7">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="3">
+        <v>3057058.43</v>
+      </c>
+      <c r="D53" s="3">
+        <v>3057058.43</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2.3851498553995043E-10</v>
+      </c>
+      <c r="F53" s="7">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="3">
         <v>0</v>
       </c>
-      <c r="C31" s="5">
+      <c r="D54" s="3">
         <v>0</v>
       </c>
-      <c r="D31" s="5">
+      <c r="E54" s="3">
         <v>0</v>
       </c>
-      <c r="E31" s="5">
+      <c r="F54" s="7">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="3">
+        <v>25613207.979999997</v>
+      </c>
+      <c r="D55" s="3">
+        <v>25613207.979999997</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1.3096723705530167E-9</v>
+      </c>
+      <c r="F55" s="7">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="3">
+        <v>3042904.43</v>
+      </c>
+      <c r="D56" s="3">
+        <v>3042904.43</v>
+      </c>
+      <c r="E56" s="3">
+        <v>5.5661075748503208E-10</v>
+      </c>
+      <c r="F56" s="7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="3">
+        <v>2176150</v>
+      </c>
+      <c r="D57" s="3">
+        <v>2176150</v>
+      </c>
+      <c r="E57" s="3">
         <v>0</v>
       </c>
-      <c r="F31" s="13">
-        <v>3801</v>
+      <c r="F57" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="3">
+        <v>415750</v>
+      </c>
+      <c r="D58" s="3">
+        <v>415750</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="3">
+        <v>3539136.0100000002</v>
+      </c>
+      <c r="D59" s="3">
+        <v>3539136.0100000002</v>
+      </c>
+      <c r="E59" s="3">
+        <v>3.3287506084889174E-10</v>
+      </c>
+      <c r="F59" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="3">
+        <v>243</v>
+      </c>
+      <c r="D60" s="3">
+        <v>243</v>
+      </c>
+      <c r="E60" s="3">
+        <v>0</v>
+      </c>
+      <c r="F60" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="3">
+        <v>558290</v>
+      </c>
+      <c r="D61" s="3">
+        <v>558290</v>
+      </c>
+      <c r="E61" s="3">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3">
+        <v>78277478.219999999</v>
+      </c>
+      <c r="D63" s="3">
+        <v>78277478.24000001</v>
+      </c>
+      <c r="E63" s="3">
+        <v>-2.0000001881271601E-2</v>
+      </c>
+      <c r="F63" s="7">
+        <v>449877</v>
       </c>
     </row>
   </sheetData>
@@ -3183,26 +3970,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="11">
-        <v>101594699</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="6">
+        <v>101726442</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11">
-        <v>101594699</v>
+      <c r="B3" s="6">
+        <v>101726442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>